<commit_message>
fixed the scheduled operations
</commit_message>
<xml_diff>
--- a/ExcelExport/Reports/query_1.xlsx
+++ b/ExcelExport/Reports/query_1.xlsx
@@ -47,13 +47,13 @@
     <t xml:space="preserve">28</t>
   </si>
   <si>
-    <t xml:space="preserve">3048</t>
+    <t xml:space="preserve">3049</t>
   </si>
   <si>
     <t xml:space="preserve">2231</t>
   </si>
   <si>
-    <t xml:space="preserve">6022</t>
+    <t xml:space="preserve">6023</t>
   </si>
   <si>
     <t xml:space="preserve">COM</t>
@@ -62,13 +62,13 @@
     <t xml:space="preserve">3</t>
   </si>
   <si>
-    <t xml:space="preserve">7523</t>
+    <t xml:space="preserve">7524</t>
   </si>
   <si>
     <t xml:space="preserve">95</t>
   </si>
   <si>
-    <t xml:space="preserve">8244</t>
+    <t xml:space="preserve">8245</t>
   </si>
   <si>
     <t xml:space="preserve">CON</t>
@@ -119,37 +119,37 @@
     <t xml:space="preserve">ESTA</t>
   </si>
   <si>
-    <t xml:space="preserve">345</t>
+    <t xml:space="preserve">346</t>
   </si>
   <si>
     <t xml:space="preserve">7</t>
   </si>
   <si>
-    <t xml:space="preserve">473</t>
+    <t xml:space="preserve">474</t>
   </si>
   <si>
     <t xml:space="preserve">FIN</t>
   </si>
   <si>
-    <t xml:space="preserve">5196</t>
+    <t xml:space="preserve">5200</t>
   </si>
   <si>
     <t xml:space="preserve">351</t>
   </si>
   <si>
-    <t xml:space="preserve">6733</t>
+    <t xml:space="preserve">6737</t>
   </si>
   <si>
     <t xml:space="preserve">INS</t>
   </si>
   <si>
-    <t xml:space="preserve">597</t>
+    <t xml:space="preserve">598</t>
   </si>
   <si>
     <t xml:space="preserve">152</t>
   </si>
   <si>
-    <t xml:space="preserve">824</t>
+    <t xml:space="preserve">825</t>
   </si>
   <si>
     <t xml:space="preserve">MAN</t>
@@ -170,13 +170,13 @@
     <t xml:space="preserve">MIN</t>
   </si>
   <si>
-    <t xml:space="preserve">718</t>
-  </si>
-  <si>
-    <t xml:space="preserve">969</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1761</t>
+    <t xml:space="preserve">719</t>
+  </si>
+  <si>
+    <t xml:space="preserve">970</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1763</t>
   </si>
   <si>
     <t xml:space="preserve">N/A</t>
@@ -191,16 +191,16 @@
     <t xml:space="preserve">1565</t>
   </si>
   <si>
-    <t xml:space="preserve">105292</t>
+    <t xml:space="preserve">105322</t>
   </si>
   <si>
     <t xml:space="preserve">496</t>
   </si>
   <si>
-    <t xml:space="preserve">20002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">155819</t>
+    <t xml:space="preserve">20003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">155850</t>
   </si>
   <si>
     <t xml:space="preserve">PROP</t>
@@ -227,16 +227,16 @@
     <t xml:space="preserve">771</t>
   </si>
   <si>
-    <t xml:space="preserve">30001</t>
+    <t xml:space="preserve">30003</t>
   </si>
   <si>
     <t xml:space="preserve">15</t>
   </si>
   <si>
-    <t xml:space="preserve">1824</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43835</t>
+    <t xml:space="preserve">1825</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43838</t>
   </si>
   <si>
     <t xml:space="preserve">SERVICES</t>
@@ -245,25 +245,25 @@
     <t xml:space="preserve">TOU</t>
   </si>
   <si>
-    <t xml:space="preserve">1598</t>
+    <t xml:space="preserve">1599</t>
   </si>
   <si>
     <t xml:space="preserve">96</t>
   </si>
   <si>
-    <t xml:space="preserve">2871</t>
+    <t xml:space="preserve">2872</t>
   </si>
   <si>
     <t xml:space="preserve">TRAN</t>
   </si>
   <si>
-    <t xml:space="preserve">1580</t>
+    <t xml:space="preserve">1581</t>
   </si>
   <si>
     <t xml:space="preserve">209</t>
   </si>
   <si>
-    <t xml:space="preserve">2466</t>
+    <t xml:space="preserve">2467</t>
   </si>
   <si>
     <t xml:space="preserve">WRTCAS</t>
@@ -275,10 +275,10 @@
     <t xml:space="preserve">16878</t>
   </si>
   <si>
-    <t xml:space="preserve">1932</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22317</t>
+    <t xml:space="preserve">1934</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22319</t>
   </si>
   <si>
     <t xml:space="preserve">financial services</t>
@@ -314,16 +314,16 @@
     <t xml:space="preserve">3089</t>
   </si>
   <si>
-    <t xml:space="preserve">196213</t>
+    <t xml:space="preserve">196256</t>
   </si>
   <si>
     <t xml:space="preserve">572</t>
   </si>
   <si>
-    <t xml:space="preserve">31196</t>
-  </si>
-  <si>
-    <t xml:space="preserve">302367</t>
+    <t xml:space="preserve">31201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">302415</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <cols>
     <col min="1" max="1" width="15.8984375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="5.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.34765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="4.34765625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="6.296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="14.09765625" bestFit="1" customWidth="1" collapsed="1"/>

</xml_diff>